<commit_message>
Update XLSX files (new column added)
</commit_message>
<xml_diff>
--- a/xlsx/α-particles.xlsx
+++ b/xlsx/α-particles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="191">
   <si>
     <t>#ExpID</t>
   </si>
@@ -791,6 +791,135 @@
   </si>
   <si>
     <t>6,41 f</t>
+  </si>
+  <si>
+    <t>Figures/Tables</t>
+  </si>
+  <si>
+    <t>Figure 2</t>
+  </si>
+  <si>
+    <t>Fig. 2C</t>
+  </si>
+  <si>
+    <t>Figure 1</t>
+  </si>
+  <si>
+    <t>Fig. 4A</t>
+  </si>
+  <si>
+    <t>Fig. 4</t>
+  </si>
+  <si>
+    <t>Table 1 &amp; Figure 1</t>
+  </si>
+  <si>
+    <t>Table 1 &amp; Figure 2</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Figure 1C</t>
+  </si>
+  <si>
+    <t>Table 3 &amp; Fig. 2b</t>
+  </si>
+  <si>
+    <t>Fig. 3a</t>
+  </si>
+  <si>
+    <t>Fig. 2</t>
+  </si>
+  <si>
+    <t>Fig. 1</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>Figure 1b</t>
+  </si>
+  <si>
+    <t>Fig. 1A</t>
+  </si>
+  <si>
+    <t>Fig. 1B</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Figure 1A &amp; Figure 1B</t>
+  </si>
+  <si>
+    <t>Figure 2 &amp; Table 1</t>
+  </si>
+  <si>
+    <t>Figure 2B</t>
+  </si>
+  <si>
+    <t>Fig. 7 &amp; Fig. 8A</t>
+  </si>
+  <si>
+    <t>Fig. 6A</t>
+  </si>
+  <si>
+    <t>Fig. 6B</t>
+  </si>
+  <si>
+    <t>Fig. 6C</t>
+  </si>
+  <si>
+    <t>Fig. 6D</t>
+  </si>
+  <si>
+    <t>Fig. 6E</t>
+  </si>
+  <si>
+    <t>Fig. 6F</t>
+  </si>
+  <si>
+    <t>Fig. 10</t>
+  </si>
+  <si>
+    <t>Figure 1A</t>
+  </si>
+  <si>
+    <t>Table 4 &amp; Fig. 5A</t>
+  </si>
+  <si>
+    <t>Fig. 3</t>
+  </si>
+  <si>
+    <t>Fig. 5</t>
+  </si>
+  <si>
+    <t>Figure 3a</t>
+  </si>
+  <si>
+    <t>Figure 5a</t>
+  </si>
+  <si>
+    <t>Figure 11 &amp; Table 1</t>
+  </si>
+  <si>
+    <t>Figure 1C &amp; Figure 2A</t>
+  </si>
+  <si>
+    <t>Figure 2A</t>
+  </si>
+  <si>
+    <t>Figure 2C</t>
+  </si>
+  <si>
+    <t>Figure 3G</t>
+  </si>
+  <si>
+    <t>Figure 1a</t>
+  </si>
+  <si>
+    <t>Figure 3A</t>
   </si>
 </sst>
 </file>
@@ -1344,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA97"/>
+  <dimension ref="A1:AB97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N83" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,24 +1489,25 @@
     <col min="6" max="6" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="3"/>
     <col min="8" max="8" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="8.5703125" style="29" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" style="38" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="3"/>
+    <col min="18" max="18" width="20.85546875" style="38" customWidth="1"/>
+    <col min="19" max="19" width="24.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1430,26 +1560,29 @@
         <v>121</v>
       </c>
       <c r="R1" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="S1" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="T1" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="U1" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="V1" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="W1" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
-    </row>
-    <row r="2" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB1" s="1"/>
+    </row>
+    <row r="2" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1498,26 +1631,29 @@
         <v>14</v>
       </c>
       <c r="R2" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="7">
+        <v>149</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="7">
         <v>23.16</v>
       </c>
-      <c r="T2" s="7">
+      <c r="U2" s="7">
         <v>115.7</v>
       </c>
-      <c r="U2" s="7">
+      <c r="V2" s="7">
         <v>24.13</v>
       </c>
-      <c r="V2" s="7">
+      <c r="W2" s="7">
         <v>112.82</v>
       </c>
-      <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
-    </row>
-    <row r="3" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB2" s="7"/>
+    </row>
+    <row r="3" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1566,9 +1702,9 @@
         <v>14</v>
       </c>
       <c r="R3" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S3" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="S3" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T3" s="7" t="s">
@@ -1580,12 +1716,15 @@
       <c r="V3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="7"/>
+      <c r="W3" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
-    </row>
-    <row r="4" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB3" s="7"/>
+    </row>
+    <row r="4" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1634,9 +1773,9 @@
         <v>14</v>
       </c>
       <c r="R4" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="S4" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T4" s="7" t="s">
@@ -1648,12 +1787,15 @@
       <c r="V4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X4" s="7"/>
+      <c r="W4" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
-    </row>
-    <row r="5" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB4" s="7"/>
+    </row>
+    <row r="5" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1702,9 +1844,9 @@
         <v>14</v>
       </c>
       <c r="R5" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="S5" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T5" s="7" t="s">
@@ -1716,12 +1858,15 @@
       <c r="V5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X5" s="7"/>
+      <c r="W5" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
-    </row>
-    <row r="6" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB5" s="7"/>
+    </row>
+    <row r="6" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1770,9 +1915,9 @@
         <v>14</v>
       </c>
       <c r="R6" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S6" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="S6" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T6" s="7" t="s">
@@ -1784,12 +1929,15 @@
       <c r="V6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X6" s="7"/>
+      <c r="W6" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB6" s="7"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1838,26 +1986,29 @@
         <v>14</v>
       </c>
       <c r="R7" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S7" s="7">
+        <v>151</v>
+      </c>
+      <c r="S7" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" s="7">
         <v>22.92</v>
       </c>
-      <c r="T7" s="7">
+      <c r="U7" s="7">
         <v>118.6</v>
       </c>
-      <c r="U7" s="12">
+      <c r="V7" s="12">
         <v>23.95</v>
       </c>
-      <c r="V7" s="12">
+      <c r="W7" s="12">
         <v>115.6</v>
       </c>
-      <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
-      <c r="Z7" s="12"/>
+      <c r="Z7" s="7"/>
       <c r="AA7" s="12"/>
-    </row>
-    <row r="8" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB7" s="12"/>
+    </row>
+    <row r="8" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1906,9 +2057,9 @@
         <v>14</v>
       </c>
       <c r="R8" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S8" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="S8" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T8" s="7" t="s">
@@ -1920,12 +2071,15 @@
       <c r="V8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X8" s="7"/>
+      <c r="W8" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
-    </row>
-    <row r="9" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB8" s="7"/>
+    </row>
+    <row r="9" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1974,9 +2128,9 @@
         <v>14</v>
       </c>
       <c r="R9" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S9" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="S9" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T9" s="7" t="s">
@@ -1988,12 +2142,15 @@
       <c r="V9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X9" s="7"/>
+      <c r="W9" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="7"/>
-    </row>
-    <row r="10" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB9" s="7"/>
+    </row>
+    <row r="10" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2042,9 +2199,9 @@
         <v>14</v>
       </c>
       <c r="R10" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S10" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="S10" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T10" s="7" t="s">
@@ -2056,12 +2213,15 @@
       <c r="V10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X10" s="7"/>
+      <c r="W10" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="7"/>
-    </row>
-    <row r="11" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB10" s="7"/>
+    </row>
+    <row r="11" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2110,9 +2270,9 @@
         <v>14</v>
       </c>
       <c r="R11" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S11" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="S11" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T11" s="7" t="s">
@@ -2124,12 +2284,15 @@
       <c r="V11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X11" s="7"/>
+      <c r="W11" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
-    </row>
-    <row r="12" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB11" s="7"/>
+    </row>
+    <row r="12" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2178,9 +2341,9 @@
         <v>14</v>
       </c>
       <c r="R12" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S12" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="S12" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T12" s="7" t="s">
@@ -2192,12 +2355,15 @@
       <c r="V12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X12" s="7"/>
+      <c r="W12" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
-    </row>
-    <row r="13" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB12" s="7"/>
+    </row>
+    <row r="13" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2246,26 +2412,29 @@
         <v>14</v>
       </c>
       <c r="R13" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S13" s="7">
+        <v>153</v>
+      </c>
+      <c r="S13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T13" s="7">
         <v>23.76</v>
       </c>
-      <c r="T13" s="7">
+      <c r="U13" s="7">
         <v>108.37</v>
       </c>
-      <c r="U13" s="7">
+      <c r="V13" s="7">
         <v>24.55</v>
       </c>
-      <c r="V13" s="7">
+      <c r="W13" s="7">
         <v>105.98</v>
       </c>
-      <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
-    </row>
-    <row r="14" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB13" s="7"/>
+    </row>
+    <row r="14" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2314,9 +2483,9 @@
         <v>14</v>
       </c>
       <c r="R14" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S14" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="S14" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T14" s="7" t="s">
@@ -2328,12 +2497,15 @@
       <c r="V14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X14" s="7"/>
+      <c r="W14" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="7"/>
-    </row>
-    <row r="15" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB14" s="7"/>
+    </row>
+    <row r="15" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2382,9 +2554,9 @@
         <v>14</v>
       </c>
       <c r="R15" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S15" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="S15" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T15" s="7" t="s">
@@ -2396,12 +2568,15 @@
       <c r="V15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X15" s="7"/>
+      <c r="W15" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="7"/>
-    </row>
-    <row r="16" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB15" s="7"/>
+    </row>
+    <row r="16" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2450,9 +2625,9 @@
         <v>14</v>
       </c>
       <c r="R16" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S16" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="S16" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T16" s="7" t="s">
@@ -2464,12 +2639,15 @@
       <c r="V16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X16" s="7"/>
+      <c r="W16" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
       <c r="AA16" s="7"/>
-    </row>
-    <row r="17" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB16" s="7"/>
+    </row>
+    <row r="17" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2518,9 +2696,9 @@
         <v>14</v>
       </c>
       <c r="R17" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S17" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="S17" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T17" s="7" t="s">
@@ -2532,12 +2710,15 @@
       <c r="V17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X17" s="7"/>
+      <c r="W17" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
-    </row>
-    <row r="18" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB17" s="7"/>
+    </row>
+    <row r="18" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2586,9 +2767,9 @@
         <v>133</v>
       </c>
       <c r="R18" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S18" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="S18" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T18" s="7" t="s">
@@ -2600,12 +2781,15 @@
       <c r="V18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X18" s="7"/>
+      <c r="W18" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
-    </row>
-    <row r="19" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB18" s="7"/>
+    </row>
+    <row r="19" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2654,9 +2838,9 @@
         <v>134</v>
       </c>
       <c r="R19" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S19" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="S19" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T19" s="7" t="s">
@@ -2668,12 +2852,15 @@
       <c r="V19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X19" s="7"/>
+      <c r="W19" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="7"/>
-    </row>
-    <row r="20" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB19" s="7"/>
+    </row>
+    <row r="20" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2722,9 +2909,9 @@
         <v>135</v>
       </c>
       <c r="R20" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S20" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="S20" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T20" s="7" t="s">
@@ -2736,12 +2923,15 @@
       <c r="V20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X20" s="7"/>
+      <c r="W20" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
       <c r="AA20" s="7"/>
-    </row>
-    <row r="21" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB20" s="7"/>
+    </row>
+    <row r="21" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2790,26 +2980,29 @@
         <v>136</v>
       </c>
       <c r="R21" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S21" s="12">
+        <v>156</v>
+      </c>
+      <c r="S21" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T21" s="12">
         <v>22.92</v>
       </c>
-      <c r="T21" s="12">
+      <c r="U21" s="12">
         <v>118.6</v>
       </c>
-      <c r="U21" s="12">
+      <c r="V21" s="12">
         <v>23.95</v>
       </c>
-      <c r="V21" s="12">
+      <c r="W21" s="12">
         <v>115.6</v>
       </c>
-      <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
-    </row>
-    <row r="22" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB21" s="12"/>
+    </row>
+    <row r="22" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2858,9 +3051,9 @@
         <v>14</v>
       </c>
       <c r="R22" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S22" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="S22" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T22" s="7" t="s">
@@ -2872,12 +3065,15 @@
       <c r="V22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X22" s="7"/>
+      <c r="W22" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
       <c r="AA22" s="7"/>
-    </row>
-    <row r="23" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB22" s="7"/>
+    </row>
+    <row r="23" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2925,10 +3121,10 @@
       <c r="Q23" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="R23" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S23" s="7" t="s">
+      <c r="R23" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="S23" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T23" s="7" t="s">
@@ -2940,12 +3136,15 @@
       <c r="V23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X23" s="7"/>
+      <c r="W23" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
       <c r="AA23" s="7"/>
-    </row>
-    <row r="24" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB23" s="7"/>
+    </row>
+    <row r="24" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2994,26 +3193,29 @@
         <v>14</v>
       </c>
       <c r="R24" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S24" s="7">
+        <v>157</v>
+      </c>
+      <c r="S24" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T24" s="7">
         <v>24.8</v>
       </c>
-      <c r="T24" s="7">
+      <c r="U24" s="7">
         <v>94.64</v>
       </c>
-      <c r="U24" s="7">
+      <c r="V24" s="7">
         <v>25.36</v>
       </c>
-      <c r="V24" s="7">
+      <c r="W24" s="7">
         <v>92.95</v>
       </c>
-      <c r="X24" s="7"/>
       <c r="Y24" s="7"/>
       <c r="Z24" s="7"/>
       <c r="AA24" s="7"/>
-    </row>
-    <row r="25" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB24" s="7"/>
+    </row>
+    <row r="25" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3062,26 +3264,29 @@
         <v>14</v>
       </c>
       <c r="R25" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S25" s="7">
+        <v>157</v>
+      </c>
+      <c r="S25" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T25" s="7">
         <v>24.8</v>
       </c>
-      <c r="T25" s="7">
+      <c r="U25" s="7">
         <v>94.64</v>
       </c>
-      <c r="U25" s="7">
+      <c r="V25" s="7">
         <v>25.36</v>
       </c>
-      <c r="V25" s="7">
+      <c r="W25" s="7">
         <v>92.95</v>
       </c>
-      <c r="X25" s="7"/>
       <c r="Y25" s="7"/>
       <c r="Z25" s="7"/>
       <c r="AA25" s="7"/>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB25" s="7"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3130,26 +3335,29 @@
         <v>14</v>
       </c>
       <c r="R26" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S26" s="7">
+        <v>158</v>
+      </c>
+      <c r="S26" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T26" s="7">
         <v>24.08</v>
       </c>
-      <c r="T26" s="7">
+      <c r="U26" s="7">
         <v>104.2</v>
       </c>
-      <c r="U26" s="7">
+      <c r="V26" s="7">
         <v>24.79</v>
       </c>
-      <c r="V26" s="7">
+      <c r="W26" s="7">
         <v>102.06</v>
       </c>
-      <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
       <c r="AA26" s="7"/>
-    </row>
-    <row r="27" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB26" s="7"/>
+    </row>
+    <row r="27" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3198,26 +3406,29 @@
         <v>14</v>
       </c>
       <c r="R27" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S27" s="7">
+        <v>159</v>
+      </c>
+      <c r="S27" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T27" s="7">
         <v>22.77</v>
       </c>
-      <c r="T27" s="7">
+      <c r="U27" s="7">
         <v>120.52</v>
       </c>
-      <c r="U27" s="7">
+      <c r="V27" s="7">
         <v>23.82</v>
       </c>
-      <c r="V27" s="7">
+      <c r="W27" s="7">
         <v>117.41</v>
       </c>
-      <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
       <c r="AA27" s="7"/>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB27" s="7"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -3266,26 +3477,29 @@
         <v>14</v>
       </c>
       <c r="R28" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S28" s="7">
+        <v>160</v>
+      </c>
+      <c r="S28" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T28" s="7">
         <v>22.16</v>
       </c>
-      <c r="T28" s="7">
+      <c r="U28" s="7">
         <v>127.33</v>
       </c>
-      <c r="U28" s="7">
+      <c r="V28" s="7">
         <v>23.41</v>
       </c>
-      <c r="V28" s="7">
+      <c r="W28" s="7">
         <v>123.76</v>
       </c>
-      <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
       <c r="AA28" s="7"/>
-    </row>
-    <row r="29" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB28" s="7"/>
+    </row>
+    <row r="29" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3334,9 +3548,9 @@
         <v>14</v>
       </c>
       <c r="R29" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S29" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="S29" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T29" s="7" t="s">
@@ -3348,12 +3562,15 @@
       <c r="V29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X29" s="7"/>
+      <c r="W29" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
       <c r="AA29" s="7"/>
-    </row>
-    <row r="30" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB29" s="7"/>
+    </row>
+    <row r="30" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -3402,26 +3619,29 @@
         <v>14</v>
       </c>
       <c r="R30" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S30" s="9">
+        <v>160</v>
+      </c>
+      <c r="S30" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T30" s="9">
         <v>21.98</v>
       </c>
-      <c r="T30" s="9">
+      <c r="U30" s="9">
         <v>130.22</v>
       </c>
-      <c r="U30" s="9">
+      <c r="V30" s="9">
         <v>23.28</v>
       </c>
-      <c r="V30" s="9">
+      <c r="W30" s="9">
         <v>126.48</v>
       </c>
-      <c r="X30" s="9"/>
       <c r="Y30" s="9"/>
       <c r="Z30" s="9"/>
       <c r="AA30" s="9"/>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB30" s="9"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -3470,9 +3690,9 @@
         <v>14</v>
       </c>
       <c r="R31" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S31" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="S31" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T31" s="7" t="s">
@@ -3484,12 +3704,15 @@
       <c r="V31" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X31" s="7"/>
+      <c r="W31" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y31" s="7"/>
       <c r="Z31" s="7"/>
       <c r="AA31" s="7"/>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB31" s="7"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3538,9 +3761,9 @@
         <v>14</v>
       </c>
       <c r="R32" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S32" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="S32" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T32" s="7" t="s">
@@ -3552,12 +3775,15 @@
       <c r="V32" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X32" s="7"/>
+      <c r="W32" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y32" s="7"/>
       <c r="Z32" s="7"/>
       <c r="AA32" s="7"/>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB32" s="7"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3606,9 +3832,9 @@
         <v>14</v>
       </c>
       <c r="R33" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S33" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="S33" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T33" s="7" t="s">
@@ -3620,12 +3846,15 @@
       <c r="V33" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X33" s="7"/>
+      <c r="W33" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y33" s="7"/>
       <c r="Z33" s="7"/>
       <c r="AA33" s="7"/>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB33" s="7"/>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -3674,9 +3903,9 @@
         <v>14</v>
       </c>
       <c r="R34" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S34" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="S34" s="32" t="s">
         <v>14</v>
       </c>
       <c r="T34" s="7" t="s">
@@ -3688,12 +3917,15 @@
       <c r="V34" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="X34" s="7"/>
+      <c r="W34" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="Y34" s="7"/>
       <c r="Z34" s="7"/>
       <c r="AA34" s="7"/>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB34" s="7"/>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -3742,26 +3974,29 @@
         <v>14</v>
       </c>
       <c r="R35" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S35" s="7">
+        <v>161</v>
+      </c>
+      <c r="S35" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T35" s="7">
         <v>25.73</v>
       </c>
-      <c r="T35" s="7">
+      <c r="U35" s="7">
         <v>83.01</v>
       </c>
-      <c r="U35" s="12">
+      <c r="V35" s="12">
         <v>26.08</v>
       </c>
-      <c r="V35" s="7">
+      <c r="W35" s="7">
         <v>81.94</v>
       </c>
-      <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
-      <c r="Z35" s="12"/>
-      <c r="AA35" s="7"/>
-    </row>
-    <row r="36" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="7"/>
+    </row>
+    <row r="36" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -3810,26 +4045,29 @@
         <v>14</v>
       </c>
       <c r="R36" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S36" s="7">
+        <v>163</v>
+      </c>
+      <c r="S36" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T36" s="7">
         <v>22.92</v>
       </c>
-      <c r="T36" s="7">
+      <c r="U36" s="7">
         <v>118.6</v>
       </c>
-      <c r="U36" s="12">
+      <c r="V36" s="12">
         <v>23.95</v>
       </c>
-      <c r="V36" s="12">
+      <c r="W36" s="12">
         <v>115.6</v>
       </c>
-      <c r="X36" s="7"/>
       <c r="Y36" s="7"/>
-      <c r="Z36" s="12"/>
+      <c r="Z36" s="7"/>
       <c r="AA36" s="12"/>
-    </row>
-    <row r="37" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB36" s="12"/>
+    </row>
+    <row r="37" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -3878,26 +4116,29 @@
         <v>14</v>
       </c>
       <c r="R37" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S37" s="7">
+        <v>163</v>
+      </c>
+      <c r="S37" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T37" s="7">
         <v>22.92</v>
       </c>
-      <c r="T37" s="7">
+      <c r="U37" s="7">
         <v>118.6</v>
       </c>
-      <c r="U37" s="12">
+      <c r="V37" s="12">
         <v>23.95</v>
       </c>
-      <c r="V37" s="12">
+      <c r="W37" s="12">
         <v>115.6</v>
       </c>
-      <c r="X37" s="7"/>
       <c r="Y37" s="7"/>
-      <c r="Z37" s="12"/>
+      <c r="Z37" s="7"/>
       <c r="AA37" s="12"/>
-    </row>
-    <row r="38" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB37" s="12"/>
+    </row>
+    <row r="38" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -3946,26 +4187,29 @@
         <v>14</v>
       </c>
       <c r="R38" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S38" s="7">
+        <v>161</v>
+      </c>
+      <c r="S38" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T38" s="7">
         <v>23.76</v>
       </c>
-      <c r="T38" s="7">
+      <c r="U38" s="7">
         <v>108.37</v>
       </c>
-      <c r="U38" s="7">
+      <c r="V38" s="7">
         <v>24.55</v>
       </c>
-      <c r="V38" s="7">
+      <c r="W38" s="7">
         <v>105.98</v>
       </c>
-      <c r="X38" s="7"/>
       <c r="Y38" s="7"/>
       <c r="Z38" s="7"/>
       <c r="AA38" s="7"/>
-    </row>
-    <row r="39" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB38" s="7"/>
+    </row>
+    <row r="39" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -4014,26 +4258,29 @@
         <v>14</v>
       </c>
       <c r="R39" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S39" s="7">
+        <v>160</v>
+      </c>
+      <c r="S39" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T39" s="7">
         <v>21.99</v>
       </c>
-      <c r="T39" s="7">
+      <c r="U39" s="7">
         <v>129.69</v>
       </c>
-      <c r="U39" s="7">
+      <c r="V39" s="7">
         <v>23.29</v>
       </c>
-      <c r="V39" s="7">
+      <c r="W39" s="7">
         <v>125.96</v>
       </c>
-      <c r="X39" s="7"/>
       <c r="Y39" s="7"/>
       <c r="Z39" s="7"/>
       <c r="AA39" s="7"/>
-    </row>
-    <row r="40" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB39" s="7"/>
+    </row>
+    <row r="40" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -4082,26 +4329,29 @@
         <v>14</v>
       </c>
       <c r="R40" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S40" s="7">
+        <v>153</v>
+      </c>
+      <c r="S40" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T40" s="7">
         <v>23.1</v>
       </c>
-      <c r="T40" s="7">
+      <c r="U40" s="7">
         <v>116.57</v>
       </c>
-      <c r="U40" s="7">
+      <c r="V40" s="7">
         <v>24.09</v>
       </c>
-      <c r="V40" s="7">
+      <c r="W40" s="7">
         <v>113.64</v>
       </c>
-      <c r="X40" s="7"/>
       <c r="Y40" s="7"/>
       <c r="Z40" s="7"/>
       <c r="AA40" s="7"/>
-    </row>
-    <row r="41" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB40" s="7"/>
+    </row>
+    <row r="41" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -4150,26 +4400,29 @@
         <v>14</v>
       </c>
       <c r="R41" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S41" s="7">
+        <v>153</v>
+      </c>
+      <c r="S41" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T41" s="7">
         <v>23.1</v>
       </c>
-      <c r="T41" s="7">
+      <c r="U41" s="7">
         <v>116.57</v>
       </c>
-      <c r="U41" s="7">
+      <c r="V41" s="7">
         <v>24.09</v>
       </c>
-      <c r="V41" s="7">
+      <c r="W41" s="7">
         <v>113.64</v>
       </c>
-      <c r="X41" s="7"/>
       <c r="Y41" s="7"/>
       <c r="Z41" s="7"/>
       <c r="AA41" s="7"/>
-    </row>
-    <row r="42" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB41" s="7"/>
+    </row>
+    <row r="42" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -4218,26 +4471,29 @@
         <v>14</v>
       </c>
       <c r="R42" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S42" s="7">
+        <v>153</v>
+      </c>
+      <c r="S42" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T42" s="7">
         <v>23.1</v>
       </c>
-      <c r="T42" s="7">
+      <c r="U42" s="7">
         <v>116.57</v>
       </c>
-      <c r="U42" s="7">
+      <c r="V42" s="7">
         <v>24.09</v>
       </c>
-      <c r="V42" s="7">
+      <c r="W42" s="7">
         <v>113.64</v>
       </c>
-      <c r="X42" s="7"/>
       <c r="Y42" s="7"/>
       <c r="Z42" s="7"/>
       <c r="AA42" s="7"/>
-    </row>
-    <row r="43" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB42" s="7"/>
+    </row>
+    <row r="43" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -4286,26 +4542,29 @@
         <v>14</v>
       </c>
       <c r="R43" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S43" s="7">
+        <v>153</v>
+      </c>
+      <c r="S43" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T43" s="7">
         <v>23.1</v>
       </c>
-      <c r="T43" s="7">
+      <c r="U43" s="7">
         <v>116.57</v>
       </c>
-      <c r="U43" s="7">
+      <c r="V43" s="7">
         <v>24.09</v>
       </c>
-      <c r="V43" s="7">
+      <c r="W43" s="7">
         <v>113.64</v>
       </c>
-      <c r="X43" s="7"/>
       <c r="Y43" s="7"/>
       <c r="Z43" s="7"/>
       <c r="AA43" s="7"/>
-    </row>
-    <row r="44" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB43" s="7"/>
+    </row>
+    <row r="44" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -4354,26 +4613,29 @@
         <v>14</v>
       </c>
       <c r="R44" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S44" s="7">
+        <v>151</v>
+      </c>
+      <c r="S44" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T44" s="7">
         <v>23.1</v>
       </c>
-      <c r="T44" s="7">
+      <c r="U44" s="7">
         <v>116.57</v>
       </c>
-      <c r="U44" s="7">
+      <c r="V44" s="7">
         <v>24.09</v>
       </c>
-      <c r="V44" s="7">
+      <c r="W44" s="7">
         <v>113.64</v>
       </c>
-      <c r="X44" s="7"/>
       <c r="Y44" s="7"/>
       <c r="Z44" s="7"/>
       <c r="AA44" s="7"/>
-    </row>
-    <row r="45" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB44" s="7"/>
+    </row>
+    <row r="45" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -4422,26 +4684,29 @@
         <v>14</v>
       </c>
       <c r="R45" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S45" s="7">
+        <v>151</v>
+      </c>
+      <c r="S45" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T45" s="7">
         <v>23.1</v>
       </c>
-      <c r="T45" s="7">
+      <c r="U45" s="7">
         <v>116.57</v>
       </c>
-      <c r="U45" s="7">
+      <c r="V45" s="7">
         <v>24.09</v>
       </c>
-      <c r="V45" s="7">
+      <c r="W45" s="7">
         <v>113.64</v>
       </c>
-      <c r="X45" s="7"/>
       <c r="Y45" s="7"/>
       <c r="Z45" s="7"/>
       <c r="AA45" s="7"/>
-    </row>
-    <row r="46" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB45" s="7"/>
+    </row>
+    <row r="46" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -4490,26 +4755,29 @@
         <v>14</v>
       </c>
       <c r="R46" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S46" s="7">
+        <v>151</v>
+      </c>
+      <c r="S46" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T46" s="7">
         <v>23.1</v>
       </c>
-      <c r="T46" s="7">
+      <c r="U46" s="7">
         <v>116.57</v>
       </c>
-      <c r="U46" s="7">
+      <c r="V46" s="7">
         <v>24.09</v>
       </c>
-      <c r="V46" s="7">
+      <c r="W46" s="7">
         <v>113.64</v>
       </c>
-      <c r="X46" s="7"/>
       <c r="Y46" s="7"/>
       <c r="Z46" s="7"/>
       <c r="AA46" s="7"/>
-    </row>
-    <row r="47" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB46" s="7"/>
+    </row>
+    <row r="47" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -4558,26 +4826,29 @@
         <v>14</v>
       </c>
       <c r="R47" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="S47" s="7">
+        <v>151</v>
+      </c>
+      <c r="S47" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="T47" s="7">
         <v>23.1</v>
       </c>
-      <c r="T47" s="7">
+      <c r="U47" s="7">
         <v>116.57</v>
       </c>
-      <c r="U47" s="7">
+      <c r="V47" s="7">
         <v>24.09</v>
       </c>
-      <c r="V47" s="7">
+      <c r="W47" s="7">
         <v>113.64</v>
       </c>
-      <c r="X47" s="7"/>
       <c r="Y47" s="7"/>
       <c r="Z47" s="7"/>
       <c r="AA47" s="7"/>
-    </row>
-    <row r="48" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB47" s="7"/>
+    </row>
+    <row r="48" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -4626,9 +4897,9 @@
         <v>14</v>
       </c>
       <c r="R48" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S48" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="S48" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T48" s="35" t="s">
@@ -4640,12 +4911,15 @@
       <c r="V48" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X48" s="18"/>
+      <c r="W48" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y48" s="18"/>
       <c r="Z48" s="18"/>
       <c r="AA48" s="18"/>
-    </row>
-    <row r="49" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB48" s="18"/>
+    </row>
+    <row r="49" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -4694,26 +4968,29 @@
         <v>14</v>
       </c>
       <c r="R49" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S49" s="36">
+        <v>151</v>
+      </c>
+      <c r="S49" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T49" s="36">
         <v>22.32</v>
       </c>
-      <c r="T49" s="36">
+      <c r="U49" s="36">
         <v>118.6</v>
       </c>
-      <c r="U49" s="36">
+      <c r="V49" s="36">
         <v>23.95</v>
       </c>
-      <c r="V49" s="36">
+      <c r="W49" s="36">
         <v>115.6</v>
       </c>
-      <c r="X49" s="19"/>
-      <c r="Y49" s="20"/>
-      <c r="Z49" s="19"/>
-      <c r="AA49" s="20"/>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Y49" s="19"/>
+      <c r="Z49" s="20"/>
+      <c r="AA49" s="19"/>
+      <c r="AB49" s="20"/>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -4762,9 +5039,9 @@
         <v>14</v>
       </c>
       <c r="R50" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S50" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="S50" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T50" s="35" t="s">
@@ -4776,12 +5053,15 @@
       <c r="V50" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X50" s="18"/>
+      <c r="W50" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y50" s="18"/>
       <c r="Z50" s="18"/>
       <c r="AA50" s="18"/>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB50" s="18"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -4830,26 +5110,29 @@
         <v>138</v>
       </c>
       <c r="R51" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S51" s="36">
+        <v>166</v>
+      </c>
+      <c r="S51" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T51" s="36">
         <v>23.1</v>
       </c>
-      <c r="T51" s="36">
+      <c r="U51" s="36">
         <v>116.57</v>
       </c>
-      <c r="U51" s="36">
+      <c r="V51" s="36">
         <v>24.09</v>
       </c>
-      <c r="V51" s="36">
+      <c r="W51" s="36">
         <v>113.64</v>
       </c>
-      <c r="X51" s="21"/>
       <c r="Y51" s="21"/>
       <c r="Z51" s="21"/>
       <c r="AA51" s="21"/>
-    </row>
-    <row r="52" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB51" s="21"/>
+    </row>
+    <row r="52" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -4898,26 +5181,29 @@
         <v>14</v>
       </c>
       <c r="R52" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S52" s="36">
+        <v>165</v>
+      </c>
+      <c r="S52" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T52" s="36">
         <v>23.22</v>
       </c>
-      <c r="T52" s="36">
+      <c r="U52" s="36">
         <v>114.51</v>
       </c>
-      <c r="U52" s="36">
+      <c r="V52" s="36">
         <v>24.16</v>
       </c>
-      <c r="V52" s="36">
+      <c r="W52" s="36">
         <v>111.72</v>
       </c>
-      <c r="X52" s="21"/>
       <c r="Y52" s="21"/>
       <c r="Z52" s="21"/>
       <c r="AA52" s="21"/>
-    </row>
-    <row r="53" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB52" s="21"/>
+    </row>
+    <row r="53" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -4966,26 +5252,29 @@
         <v>139</v>
       </c>
       <c r="R53" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S53" s="36">
+        <v>167</v>
+      </c>
+      <c r="S53" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T53" s="36">
         <v>21.98</v>
       </c>
-      <c r="T53" s="36">
+      <c r="U53" s="36">
         <v>130.22</v>
       </c>
-      <c r="U53" s="36">
+      <c r="V53" s="36">
         <v>23.28</v>
       </c>
-      <c r="V53" s="36">
+      <c r="W53" s="36">
         <v>126.49</v>
       </c>
-      <c r="X53" s="21"/>
       <c r="Y53" s="21"/>
       <c r="Z53" s="21"/>
       <c r="AA53" s="21"/>
-    </row>
-    <row r="54" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB53" s="21"/>
+    </row>
+    <row r="54" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -5034,26 +5323,29 @@
         <v>14</v>
       </c>
       <c r="R54" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S54" s="36">
+        <v>160</v>
+      </c>
+      <c r="S54" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T54" s="36">
         <v>22.26</v>
       </c>
-      <c r="T54" s="36">
+      <c r="U54" s="36">
         <v>126.46</v>
       </c>
-      <c r="U54" s="36">
+      <c r="V54" s="36">
         <v>23.49</v>
       </c>
-      <c r="V54" s="36">
+      <c r="W54" s="36">
         <v>122.94</v>
       </c>
-      <c r="X54" s="21"/>
       <c r="Y54" s="21"/>
       <c r="Z54" s="21"/>
       <c r="AA54" s="21"/>
-    </row>
-    <row r="55" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB54" s="21"/>
+    </row>
+    <row r="55" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -5102,26 +5394,29 @@
         <v>14</v>
       </c>
       <c r="R55" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S55" s="36">
+        <v>160</v>
+      </c>
+      <c r="S55" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T55" s="36">
         <v>22.26</v>
       </c>
-      <c r="T55" s="36">
+      <c r="U55" s="36">
         <v>126.46</v>
       </c>
-      <c r="U55" s="36">
+      <c r="V55" s="36">
         <v>23.49</v>
       </c>
-      <c r="V55" s="36">
+      <c r="W55" s="36">
         <v>122.94</v>
       </c>
-      <c r="X55" s="21"/>
       <c r="Y55" s="21"/>
       <c r="Z55" s="21"/>
       <c r="AA55" s="21"/>
-    </row>
-    <row r="56" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB55" s="21"/>
+    </row>
+    <row r="56" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -5170,26 +5465,29 @@
         <v>14</v>
       </c>
       <c r="R56" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S56" s="36">
+        <v>160</v>
+      </c>
+      <c r="S56" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T56" s="36">
         <v>22.26</v>
       </c>
-      <c r="T56" s="36">
+      <c r="U56" s="36">
         <v>126.46</v>
       </c>
-      <c r="U56" s="36">
+      <c r="V56" s="36">
         <v>23.49</v>
       </c>
-      <c r="V56" s="36">
+      <c r="W56" s="36">
         <v>122.94</v>
       </c>
-      <c r="X56" s="21"/>
       <c r="Y56" s="21"/>
       <c r="Z56" s="21"/>
       <c r="AA56" s="21"/>
-    </row>
-    <row r="57" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB56" s="21"/>
+    </row>
+    <row r="57" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -5238,26 +5536,29 @@
         <v>14</v>
       </c>
       <c r="R57" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S57" s="36">
+        <v>160</v>
+      </c>
+      <c r="S57" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T57" s="36">
         <v>22.26</v>
       </c>
-      <c r="T57" s="36">
+      <c r="U57" s="36">
         <v>126.46</v>
       </c>
-      <c r="U57" s="36">
+      <c r="V57" s="36">
         <v>23.49</v>
       </c>
-      <c r="V57" s="36">
+      <c r="W57" s="36">
         <v>122.94</v>
       </c>
-      <c r="X57" s="21"/>
       <c r="Y57" s="21"/>
       <c r="Z57" s="21"/>
       <c r="AA57" s="21"/>
-    </row>
-    <row r="58" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB57" s="21"/>
+    </row>
+    <row r="58" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -5306,26 +5607,29 @@
         <v>14</v>
       </c>
       <c r="R58" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S58" s="36">
+        <v>160</v>
+      </c>
+      <c r="S58" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T58" s="36">
         <v>22.26</v>
       </c>
-      <c r="T58" s="36">
+      <c r="U58" s="36">
         <v>126.46</v>
       </c>
-      <c r="U58" s="36">
+      <c r="V58" s="36">
         <v>23.49</v>
       </c>
-      <c r="V58" s="36">
+      <c r="W58" s="36">
         <v>122.94</v>
       </c>
-      <c r="X58" s="21"/>
       <c r="Y58" s="21"/>
       <c r="Z58" s="21"/>
       <c r="AA58" s="21"/>
-    </row>
-    <row r="59" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB58" s="21"/>
+    </row>
+    <row r="59" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -5374,26 +5678,29 @@
         <v>14</v>
       </c>
       <c r="R59" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S59" s="36">
+        <v>160</v>
+      </c>
+      <c r="S59" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T59" s="36">
         <v>22.26</v>
       </c>
-      <c r="T59" s="36">
+      <c r="U59" s="36">
         <v>126.46</v>
       </c>
-      <c r="U59" s="36">
+      <c r="V59" s="36">
         <v>23.49</v>
       </c>
-      <c r="V59" s="36">
+      <c r="W59" s="36">
         <v>122.94</v>
       </c>
-      <c r="X59" s="21"/>
       <c r="Y59" s="21"/>
       <c r="Z59" s="21"/>
       <c r="AA59" s="21"/>
-    </row>
-    <row r="60" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB59" s="21"/>
+    </row>
+    <row r="60" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -5442,26 +5749,29 @@
         <v>140</v>
       </c>
       <c r="R60" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S60" s="36">
+        <v>168</v>
+      </c>
+      <c r="S60" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T60" s="36">
         <v>21.98</v>
       </c>
-      <c r="T60" s="36">
+      <c r="U60" s="36">
         <v>130.22</v>
       </c>
-      <c r="U60" s="36">
+      <c r="V60" s="36">
         <v>23.28</v>
       </c>
-      <c r="V60" s="36">
+      <c r="W60" s="36">
         <v>126.48</v>
       </c>
-      <c r="X60" s="21"/>
       <c r="Y60" s="21"/>
       <c r="Z60" s="21"/>
       <c r="AA60" s="21"/>
-    </row>
-    <row r="61" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB60" s="21"/>
+    </row>
+    <row r="61" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -5510,26 +5820,29 @@
         <v>14</v>
       </c>
       <c r="R61" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S61" s="36">
+        <v>169</v>
+      </c>
+      <c r="S61" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T61" s="36">
         <v>23.76</v>
       </c>
-      <c r="T61" s="36">
+      <c r="U61" s="36">
         <v>108.37</v>
       </c>
-      <c r="U61" s="36">
+      <c r="V61" s="36">
         <v>24.55</v>
       </c>
-      <c r="V61" s="36">
+      <c r="W61" s="36">
         <v>105.98</v>
       </c>
-      <c r="X61" s="21"/>
       <c r="Y61" s="21"/>
       <c r="Z61" s="21"/>
       <c r="AA61" s="21"/>
-    </row>
-    <row r="62" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB61" s="21"/>
+    </row>
+    <row r="62" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -5578,9 +5891,9 @@
         <v>14</v>
       </c>
       <c r="R62" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S62" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="S62" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T62" s="35" t="s">
@@ -5592,12 +5905,15 @@
       <c r="V62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X62" s="18"/>
+      <c r="W62" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y62" s="18"/>
       <c r="Z62" s="18"/>
       <c r="AA62" s="18"/>
-    </row>
-    <row r="63" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB62" s="18"/>
+    </row>
+    <row r="63" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -5646,9 +5962,9 @@
         <v>14</v>
       </c>
       <c r="R63" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S63" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="S63" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T63" s="35" t="s">
@@ -5660,12 +5976,15 @@
       <c r="V63" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X63" s="18"/>
+      <c r="W63" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y63" s="18"/>
       <c r="Z63" s="18"/>
       <c r="AA63" s="18"/>
-    </row>
-    <row r="64" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB63" s="18"/>
+    </row>
+    <row r="64" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -5714,26 +6033,29 @@
         <v>14</v>
       </c>
       <c r="R64" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S64" s="36">
+        <v>151</v>
+      </c>
+      <c r="S64" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T64" s="36">
         <v>23.16</v>
       </c>
-      <c r="T64" s="36">
+      <c r="U64" s="36">
         <v>115.7</v>
       </c>
-      <c r="U64" s="36">
+      <c r="V64" s="36">
         <v>24.13</v>
       </c>
-      <c r="V64" s="36">
+      <c r="W64" s="36">
         <v>112.82</v>
       </c>
-      <c r="X64" s="21"/>
       <c r="Y64" s="21"/>
       <c r="Z64" s="21"/>
       <c r="AA64" s="21"/>
-    </row>
-    <row r="65" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB64" s="21"/>
+    </row>
+    <row r="65" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -5782,9 +6104,9 @@
         <v>14</v>
       </c>
       <c r="R65" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S65" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="S65" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T65" s="35" t="s">
@@ -5796,12 +6118,15 @@
       <c r="V65" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X65" s="18"/>
+      <c r="W65" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y65" s="18"/>
       <c r="Z65" s="18"/>
       <c r="AA65" s="18"/>
-    </row>
-    <row r="66" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB65" s="18"/>
+    </row>
+    <row r="66" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -5849,27 +6174,30 @@
       <c r="Q66" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="R66" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S66" s="35">
+      <c r="R66" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="S66" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T66" s="35">
         <v>27.16</v>
       </c>
-      <c r="T66" s="35">
+      <c r="U66" s="35">
         <v>62.33</v>
       </c>
-      <c r="U66" s="35">
+      <c r="V66" s="35">
         <v>27.27</v>
       </c>
-      <c r="V66" s="35">
+      <c r="W66" s="35">
         <v>62</v>
       </c>
-      <c r="X66" s="18"/>
       <c r="Y66" s="18"/>
-      <c r="Z66" s="23"/>
-      <c r="AA66" s="18"/>
-    </row>
-    <row r="67" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="Z66" s="18"/>
+      <c r="AA66" s="23"/>
+      <c r="AB66" s="18"/>
+    </row>
+    <row r="67" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -5918,26 +6246,29 @@
         <v>14</v>
       </c>
       <c r="R67" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S67" s="36">
+        <v>171</v>
+      </c>
+      <c r="S67" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T67" s="36">
         <v>23.22</v>
       </c>
-      <c r="T67" s="36">
+      <c r="U67" s="36">
         <v>114.51</v>
       </c>
-      <c r="U67" s="36">
+      <c r="V67" s="36">
         <v>24.16</v>
       </c>
-      <c r="V67" s="36">
+      <c r="W67" s="36">
         <v>111.72</v>
       </c>
-      <c r="X67" s="21"/>
       <c r="Y67" s="21"/>
       <c r="Z67" s="21"/>
       <c r="AA67" s="21"/>
-    </row>
-    <row r="68" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB67" s="21"/>
+    </row>
+    <row r="68" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -5986,26 +6317,29 @@
         <v>14</v>
       </c>
       <c r="R68" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S68" s="36">
+        <v>172</v>
+      </c>
+      <c r="S68" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T68" s="36">
         <v>23.22</v>
       </c>
-      <c r="T68" s="36">
+      <c r="U68" s="36">
         <v>114.51</v>
       </c>
-      <c r="U68" s="36">
+      <c r="V68" s="36">
         <v>24.16</v>
       </c>
-      <c r="V68" s="36">
+      <c r="W68" s="36">
         <v>111.72</v>
       </c>
-      <c r="X68" s="21"/>
       <c r="Y68" s="21"/>
       <c r="Z68" s="21"/>
       <c r="AA68" s="21"/>
-    </row>
-    <row r="69" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB68" s="21"/>
+    </row>
+    <row r="69" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -6054,26 +6388,29 @@
         <v>14</v>
       </c>
       <c r="R69" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S69" s="36">
+        <v>173</v>
+      </c>
+      <c r="S69" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T69" s="36">
         <v>23.22</v>
       </c>
-      <c r="T69" s="36">
+      <c r="U69" s="36">
         <v>114.51</v>
       </c>
-      <c r="U69" s="36">
+      <c r="V69" s="36">
         <v>24.16</v>
       </c>
-      <c r="V69" s="36">
+      <c r="W69" s="36">
         <v>111.72</v>
       </c>
-      <c r="X69" s="21"/>
       <c r="Y69" s="21"/>
       <c r="Z69" s="21"/>
       <c r="AA69" s="21"/>
-    </row>
-    <row r="70" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB69" s="21"/>
+    </row>
+    <row r="70" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -6122,26 +6459,29 @@
         <v>14</v>
       </c>
       <c r="R70" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S70" s="36">
+        <v>174</v>
+      </c>
+      <c r="S70" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T70" s="36">
         <v>23.22</v>
       </c>
-      <c r="T70" s="36">
+      <c r="U70" s="36">
         <v>114.51</v>
       </c>
-      <c r="U70" s="36">
+      <c r="V70" s="36">
         <v>24.16</v>
       </c>
-      <c r="V70" s="36">
+      <c r="W70" s="36">
         <v>111.72</v>
       </c>
-      <c r="X70" s="21"/>
       <c r="Y70" s="21"/>
       <c r="Z70" s="21"/>
       <c r="AA70" s="21"/>
-    </row>
-    <row r="71" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB70" s="21"/>
+    </row>
+    <row r="71" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -6190,26 +6530,29 @@
         <v>14</v>
       </c>
       <c r="R71" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S71" s="36">
+        <v>175</v>
+      </c>
+      <c r="S71" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T71" s="36">
         <v>23.22</v>
       </c>
-      <c r="T71" s="36">
+      <c r="U71" s="36">
         <v>114.51</v>
       </c>
-      <c r="U71" s="36">
+      <c r="V71" s="36">
         <v>24.16</v>
       </c>
-      <c r="V71" s="36">
+      <c r="W71" s="36">
         <v>111.72</v>
       </c>
-      <c r="X71" s="21"/>
       <c r="Y71" s="21"/>
       <c r="Z71" s="21"/>
       <c r="AA71" s="21"/>
-    </row>
-    <row r="72" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB71" s="21"/>
+    </row>
+    <row r="72" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -6258,26 +6601,29 @@
         <v>14</v>
       </c>
       <c r="R72" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S72" s="36">
+        <v>176</v>
+      </c>
+      <c r="S72" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T72" s="36">
         <v>23.22</v>
       </c>
-      <c r="T72" s="36">
+      <c r="U72" s="36">
         <v>114.51</v>
       </c>
-      <c r="U72" s="36">
+      <c r="V72" s="36">
         <v>24.16</v>
       </c>
-      <c r="V72" s="36">
+      <c r="W72" s="36">
         <v>111.72</v>
       </c>
-      <c r="X72" s="21"/>
       <c r="Y72" s="21"/>
       <c r="Z72" s="21"/>
       <c r="AA72" s="21"/>
-    </row>
-    <row r="73" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB72" s="21"/>
+    </row>
+    <row r="73" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -6326,9 +6672,9 @@
         <v>14</v>
       </c>
       <c r="R73" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S73" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="S73" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T73" s="35" t="s">
@@ -6340,12 +6686,15 @@
       <c r="V73" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X73" s="18"/>
+      <c r="W73" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y73" s="18"/>
       <c r="Z73" s="18"/>
       <c r="AA73" s="18"/>
-    </row>
-    <row r="74" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB73" s="18"/>
+    </row>
+    <row r="74" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -6394,9 +6743,9 @@
         <v>14</v>
       </c>
       <c r="R74" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S74" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="S74" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T74" s="35" t="s">
@@ -6408,12 +6757,15 @@
       <c r="V74" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X74" s="18"/>
+      <c r="W74" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y74" s="18"/>
       <c r="Z74" s="18"/>
       <c r="AA74" s="18"/>
-    </row>
-    <row r="75" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB74" s="18"/>
+    </row>
+    <row r="75" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -6462,9 +6814,9 @@
         <v>14</v>
       </c>
       <c r="R75" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S75" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="S75" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T75" s="35" t="s">
@@ -6476,12 +6828,15 @@
       <c r="V75" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X75" s="18"/>
+      <c r="W75" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y75" s="18"/>
       <c r="Z75" s="18"/>
       <c r="AA75" s="18"/>
-    </row>
-    <row r="76" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB75" s="18"/>
+    </row>
+    <row r="76" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -6529,10 +6884,10 @@
       <c r="Q76" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="R76" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S76" s="35" t="s">
+      <c r="R76" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="S76" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T76" s="35" t="s">
@@ -6544,12 +6899,15 @@
       <c r="V76" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X76" s="18"/>
+      <c r="W76" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y76" s="18"/>
       <c r="Z76" s="18"/>
       <c r="AA76" s="18"/>
-    </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB76" s="18"/>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -6598,9 +6956,9 @@
         <v>14</v>
       </c>
       <c r="R77" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S77" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="S77" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T77" s="35" t="s">
@@ -6612,12 +6970,15 @@
       <c r="V77" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X77" s="18"/>
+      <c r="W77" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y77" s="18"/>
       <c r="Z77" s="18"/>
       <c r="AA77" s="18"/>
-    </row>
-    <row r="78" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB77" s="18"/>
+    </row>
+    <row r="78" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -6666,9 +7027,9 @@
         <v>14</v>
       </c>
       <c r="R78" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S78" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="S78" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T78" s="35" t="s">
@@ -6680,12 +7041,15 @@
       <c r="V78" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X78" s="18"/>
+      <c r="W78" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y78" s="18"/>
       <c r="Z78" s="18"/>
       <c r="AA78" s="18"/>
-    </row>
-    <row r="79" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB78" s="18"/>
+    </row>
+    <row r="79" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -6734,9 +7098,9 @@
         <v>14</v>
       </c>
       <c r="R79" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S79" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="S79" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T79" s="35" t="s">
@@ -6748,12 +7112,15 @@
       <c r="V79" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X79" s="18"/>
+      <c r="W79" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y79" s="18"/>
       <c r="Z79" s="18"/>
       <c r="AA79" s="18"/>
-    </row>
-    <row r="80" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB79" s="18"/>
+    </row>
+    <row r="80" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -6802,9 +7169,9 @@
         <v>14</v>
       </c>
       <c r="R80" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S80" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="S80" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T80" s="35" t="s">
@@ -6816,12 +7183,15 @@
       <c r="V80" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X80" s="18"/>
+      <c r="W80" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y80" s="18"/>
       <c r="Z80" s="18"/>
       <c r="AA80" s="18"/>
-    </row>
-    <row r="81" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB80" s="18"/>
+    </row>
+    <row r="81" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -6870,9 +7240,9 @@
         <v>14</v>
       </c>
       <c r="R81" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S81" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="S81" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T81" s="35" t="s">
@@ -6884,12 +7254,15 @@
       <c r="V81" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X81" s="18"/>
+      <c r="W81" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y81" s="18"/>
       <c r="Z81" s="18"/>
       <c r="AA81" s="18"/>
-    </row>
-    <row r="82" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB81" s="18"/>
+    </row>
+    <row r="82" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -6938,26 +7311,29 @@
         <v>14</v>
       </c>
       <c r="R82" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S82" s="35">
+        <v>161</v>
+      </c>
+      <c r="S82" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T82" s="35">
         <v>24.08</v>
       </c>
-      <c r="T82" s="35">
+      <c r="U82" s="35">
         <v>104.2</v>
       </c>
-      <c r="U82" s="35">
+      <c r="V82" s="35">
         <v>24.79</v>
       </c>
-      <c r="V82" s="35">
+      <c r="W82" s="35">
         <v>102.06</v>
       </c>
-      <c r="X82" s="18"/>
       <c r="Y82" s="18"/>
       <c r="Z82" s="18"/>
       <c r="AA82" s="18"/>
-    </row>
-    <row r="83" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB82" s="18"/>
+    </row>
+    <row r="83" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -7006,26 +7382,29 @@
         <v>14</v>
       </c>
       <c r="R83" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S83" s="35">
+        <v>161</v>
+      </c>
+      <c r="S83" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T83" s="35">
         <v>24.08</v>
       </c>
-      <c r="T83" s="35">
+      <c r="U83" s="35">
         <v>104.2</v>
       </c>
-      <c r="U83" s="35">
+      <c r="V83" s="35">
         <v>24.79</v>
       </c>
-      <c r="V83" s="35">
+      <c r="W83" s="35">
         <v>102.06</v>
       </c>
-      <c r="X83" s="18"/>
       <c r="Y83" s="18"/>
       <c r="Z83" s="18"/>
       <c r="AA83" s="18"/>
-    </row>
-    <row r="84" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB83" s="18"/>
+    </row>
+    <row r="84" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -7073,10 +7452,10 @@
       <c r="Q84" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="R84" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S84" s="35" t="s">
+      <c r="R84" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="S84" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T84" s="35" t="s">
@@ -7088,12 +7467,15 @@
       <c r="V84" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X84" s="18"/>
+      <c r="W84" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y84" s="18"/>
       <c r="Z84" s="18"/>
       <c r="AA84" s="18"/>
-    </row>
-    <row r="85" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB84" s="18"/>
+    </row>
+    <row r="85" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -7141,10 +7523,10 @@
       <c r="Q85" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="R85" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S85" s="35" t="s">
+      <c r="R85" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="S85" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T85" s="35" t="s">
@@ -7156,12 +7538,15 @@
       <c r="V85" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X85" s="18"/>
+      <c r="W85" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y85" s="18"/>
       <c r="Z85" s="18"/>
       <c r="AA85" s="18"/>
-    </row>
-    <row r="86" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB85" s="18"/>
+    </row>
+    <row r="86" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -7210,9 +7595,9 @@
         <v>14</v>
       </c>
       <c r="R86" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S86" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="S86" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T86" s="35" t="s">
@@ -7224,12 +7609,15 @@
       <c r="V86" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X86" s="18"/>
+      <c r="W86" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y86" s="18"/>
       <c r="Z86" s="18"/>
       <c r="AA86" s="18"/>
-    </row>
-    <row r="87" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB86" s="18"/>
+    </row>
+    <row r="87" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -7277,27 +7665,30 @@
       <c r="Q87" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="R87" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S87" s="35">
+      <c r="R87" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="S87" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T87" s="35">
         <v>21.2</v>
       </c>
-      <c r="T87" s="35">
+      <c r="U87" s="35">
         <v>139.22999999999999</v>
       </c>
-      <c r="U87" s="35">
+      <c r="V87" s="35">
         <v>22.72</v>
       </c>
-      <c r="V87" s="35">
+      <c r="W87" s="35">
         <v>135.02000000000001</v>
       </c>
-      <c r="X87" s="18"/>
       <c r="Y87" s="18"/>
       <c r="Z87" s="18"/>
       <c r="AA87" s="18"/>
-    </row>
-    <row r="88" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB87" s="18"/>
+    </row>
+    <row r="88" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -7345,10 +7736,10 @@
       <c r="Q88" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="R88" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S88" s="35" t="s">
+      <c r="R88" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="S88" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T88" s="35" t="s">
@@ -7360,12 +7751,15 @@
       <c r="V88" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X88" s="18"/>
+      <c r="W88" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y88" s="18"/>
       <c r="Z88" s="18"/>
       <c r="AA88" s="18"/>
-    </row>
-    <row r="89" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB88" s="18"/>
+    </row>
+    <row r="89" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -7413,10 +7807,10 @@
       <c r="Q89" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="R89" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S89" s="35" t="s">
+      <c r="R89" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="S89" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T89" s="35" t="s">
@@ -7428,12 +7822,15 @@
       <c r="V89" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X89" s="18"/>
+      <c r="W89" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y89" s="18"/>
       <c r="Z89" s="18"/>
       <c r="AA89" s="18"/>
-    </row>
-    <row r="90" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB89" s="18"/>
+    </row>
+    <row r="90" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -7481,10 +7878,10 @@
       <c r="Q90" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="R90" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S90" s="35" t="s">
+      <c r="R90" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="S90" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T90" s="35" t="s">
@@ -7496,12 +7893,15 @@
       <c r="V90" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X90" s="18"/>
+      <c r="W90" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y90" s="18"/>
       <c r="Z90" s="18"/>
       <c r="AA90" s="18"/>
-    </row>
-    <row r="91" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB90" s="18"/>
+    </row>
+    <row r="91" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -7550,9 +7950,9 @@
         <v>14</v>
       </c>
       <c r="R91" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S91" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="S91" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T91" s="35" t="s">
@@ -7564,12 +7964,15 @@
       <c r="V91" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X91" s="18"/>
+      <c r="W91" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y91" s="18"/>
       <c r="Z91" s="18"/>
       <c r="AA91" s="18"/>
-    </row>
-    <row r="92" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB91" s="18"/>
+    </row>
+    <row r="92" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -7618,26 +8021,29 @@
         <v>14</v>
       </c>
       <c r="R92" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S92" s="36">
+        <v>189</v>
+      </c>
+      <c r="S92" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T92" s="36">
         <v>22.32</v>
       </c>
-      <c r="T92" s="35">
+      <c r="U92" s="35">
         <v>118.6</v>
       </c>
-      <c r="U92" s="35">
+      <c r="V92" s="35">
         <v>23.95</v>
       </c>
-      <c r="V92" s="35">
+      <c r="W92" s="35">
         <v>115.66</v>
       </c>
-      <c r="X92" s="19"/>
-      <c r="Y92" s="18"/>
+      <c r="Y92" s="19"/>
       <c r="Z92" s="18"/>
       <c r="AA92" s="18"/>
-    </row>
-    <row r="93" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB92" s="18"/>
+    </row>
+    <row r="93" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -7686,26 +8092,29 @@
         <v>14</v>
       </c>
       <c r="R93" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S93" s="36">
+        <v>163</v>
+      </c>
+      <c r="S93" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T93" s="36">
         <v>22.32</v>
       </c>
-      <c r="T93" s="35">
+      <c r="U93" s="35">
         <v>118.6</v>
       </c>
-      <c r="U93" s="35">
+      <c r="V93" s="35">
         <v>23.95</v>
       </c>
-      <c r="V93" s="35">
+      <c r="W93" s="35">
         <v>115.66</v>
       </c>
-      <c r="X93" s="19"/>
-      <c r="Y93" s="18"/>
+      <c r="Y93" s="19"/>
       <c r="Z93" s="18"/>
       <c r="AA93" s="18"/>
-    </row>
-    <row r="94" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB93" s="18"/>
+    </row>
+    <row r="94" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -7754,9 +8163,9 @@
         <v>14</v>
       </c>
       <c r="R94" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S94" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="S94" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T94" s="35" t="s">
@@ -7768,12 +8177,15 @@
       <c r="V94" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X94" s="18"/>
+      <c r="W94" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y94" s="18"/>
       <c r="Z94" s="18"/>
       <c r="AA94" s="18"/>
-    </row>
-    <row r="95" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB94" s="18"/>
+    </row>
+    <row r="95" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -7822,9 +8234,9 @@
         <v>14</v>
       </c>
       <c r="R95" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S95" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="S95" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T95" s="35" t="s">
@@ -7836,12 +8248,15 @@
       <c r="V95" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X95" s="18"/>
+      <c r="W95" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y95" s="18"/>
       <c r="Z95" s="18"/>
       <c r="AA95" s="18"/>
-    </row>
-    <row r="96" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB95" s="18"/>
+    </row>
+    <row r="96" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -7890,9 +8305,9 @@
         <v>14</v>
       </c>
       <c r="R96" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S96" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="S96" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T96" s="35" t="s">
@@ -7904,12 +8319,15 @@
       <c r="V96" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X96" s="18"/>
+      <c r="W96" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y96" s="18"/>
       <c r="Z96" s="18"/>
       <c r="AA96" s="18"/>
-    </row>
-    <row r="97" spans="1:27" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="AB96" s="18"/>
+    </row>
+    <row r="97" spans="1:28" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -7958,9 +8376,9 @@
         <v>14</v>
       </c>
       <c r="R97" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="S97" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="S97" s="34" t="s">
         <v>14</v>
       </c>
       <c r="T97" s="35" t="s">
@@ -7972,10 +8390,13 @@
       <c r="V97" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X97" s="18"/>
+      <c r="W97" s="35" t="s">
+        <v>14</v>
+      </c>
       <c r="Y97" s="18"/>
       <c r="Z97" s="18"/>
       <c r="AA97" s="18"/>
+      <c r="AB97" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>